<commit_message>
Actualización Documento Historias de Usuario
Se modificaron los códicos correspondientes a las Historias de Usuario.
</commit_message>
<xml_diff>
--- a/HU-HistoriaDeUsuario-HotelCeleste17062019.xlsx
+++ b/HU-HistoriaDeUsuario-HotelCeleste17062019.xlsx
@@ -573,11 +573,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-409036608"/>
-        <c:axId val="-409036064"/>
+        <c:axId val="276822736"/>
+        <c:axId val="276811856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-409036608"/>
+        <c:axId val="276822736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,7 +587,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-409036064"/>
+        <c:crossAx val="276811856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -595,7 +595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-409036064"/>
+        <c:axId val="276811856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -606,7 +606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-409036608"/>
+        <c:crossAx val="276822736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,8 +987,8 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1038,33 +1038,33 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>46</v>
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="164.25" customHeight="1">
+        <v>31</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="250.5" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="201.75" customHeight="1">
@@ -1072,16 +1072,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="E5" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="141.75" customHeight="1">
@@ -1089,13 +1089,13 @@
         <v>41</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>40</v>
@@ -1106,16 +1106,16 @@
         <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="4">
-        <v>2</v>
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="156" customHeight="1">

</xml_diff>